<commit_message>
ensure first worksheet is selected
</commit_message>
<xml_diff>
--- a/te_algorithms/data/summary_table_drought.xlsx
+++ b/te_algorithms/data/summary_table_drought.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\LandDegradation\trends.earth\LDMP\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\LandDegradation\trends.earth-prais-prep\docker\summary_worker\trends.earth-algorithms\te_algorithms\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAA2A74B-0640-4F9C-9F7F-4BBD4639A8A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C87C84FB-E731-4EF2-88B3-9BA96DD0FD76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4875" yWindow="1920" windowWidth="28065" windowHeight="17250" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Area under drought by year" sheetId="11" r:id="rId1"/>
@@ -474,6 +474,24 @@
     <xf numFmtId="10" fontId="0" fillId="4" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -487,25 +505,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -835,9 +835,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD4BB6A9-A36E-4038-9A88-A1EAFF46FB3F}">
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="96" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -870,53 +868,53 @@
       </c>
     </row>
     <row r="3" spans="1:15" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="40"/>
-      <c r="K3" s="40"/>
-      <c r="L3" s="40"/>
-      <c r="M3" s="40"/>
-      <c r="N3" s="40"/>
-      <c r="O3" s="40"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
+      <c r="N3" s="38"/>
+      <c r="O3" s="38"/>
     </row>
     <row r="4" spans="1:15" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5"/>
     </row>
     <row r="5" spans="1:15" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
-      <c r="D5" s="41" t="s">
+      <c r="D5" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="42"/>
-      <c r="F5" s="41" t="s">
+      <c r="E5" s="40"/>
+      <c r="F5" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="42"/>
-      <c r="H5" s="41" t="s">
+      <c r="G5" s="40"/>
+      <c r="H5" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="42"/>
-      <c r="J5" s="41" t="s">
+      <c r="I5" s="40"/>
+      <c r="J5" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="42"/>
-      <c r="L5" s="41" t="s">
+      <c r="K5" s="40"/>
+      <c r="L5" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="M5" s="42"/>
-      <c r="N5" s="38" t="s">
+      <c r="M5" s="40"/>
+      <c r="N5" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="O5" s="39"/>
+      <c r="O5" s="45"/>
     </row>
     <row r="6" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="16" t="s">
@@ -963,7 +961,7 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="35"/>
+      <c r="A7" s="41"/>
       <c r="B7" s="17"/>
       <c r="C7" s="21" t="str">
         <f>IF(ISBLANK($B7),"",SUM(D7,F7,H7,J7,L7,N7))</f>
@@ -1001,7 +999,7 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="35"/>
+      <c r="A8" s="41"/>
       <c r="B8" s="17"/>
       <c r="C8" s="21" t="str">
         <f t="shared" ref="C8:C29" si="0">IF(ISBLANK($B8),"",SUM(D8,F8,H8,J8,L8,N8))</f>
@@ -1039,7 +1037,7 @@
       </c>
     </row>
     <row r="9" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="35"/>
+      <c r="A9" s="41"/>
       <c r="B9" s="17"/>
       <c r="C9" s="21" t="str">
         <f t="shared" si="0"/>
@@ -1077,7 +1075,7 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="35"/>
+      <c r="A10" s="41"/>
       <c r="B10" s="17"/>
       <c r="C10" s="21" t="str">
         <f t="shared" si="0"/>
@@ -1115,7 +1113,7 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="35"/>
+      <c r="A11" s="41"/>
       <c r="B11" s="17"/>
       <c r="C11" s="21" t="str">
         <f t="shared" si="0"/>
@@ -1153,7 +1151,7 @@
       </c>
     </row>
     <row r="12" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="35"/>
+      <c r="A12" s="41"/>
       <c r="B12" s="17"/>
       <c r="C12" s="21" t="str">
         <f t="shared" si="0"/>
@@ -1191,7 +1189,7 @@
       </c>
     </row>
     <row r="13" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="35"/>
+      <c r="A13" s="41"/>
       <c r="B13" s="17"/>
       <c r="C13" s="21" t="str">
         <f t="shared" si="0"/>
@@ -1229,7 +1227,7 @@
       </c>
     </row>
     <row r="14" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="35"/>
+      <c r="A14" s="41"/>
       <c r="B14" s="17"/>
       <c r="C14" s="21" t="str">
         <f t="shared" si="0"/>
@@ -1267,7 +1265,7 @@
       </c>
     </row>
     <row r="15" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="35"/>
+      <c r="A15" s="41"/>
       <c r="B15" s="17"/>
       <c r="C15" s="21" t="str">
         <f t="shared" si="0"/>
@@ -1305,7 +1303,7 @@
       </c>
     </row>
     <row r="16" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="35"/>
+      <c r="A16" s="41"/>
       <c r="B16" s="17"/>
       <c r="C16" s="21" t="str">
         <f t="shared" si="0"/>
@@ -1343,7 +1341,7 @@
       </c>
     </row>
     <row r="17" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="35"/>
+      <c r="A17" s="41"/>
       <c r="B17" s="17"/>
       <c r="C17" s="21" t="str">
         <f t="shared" si="0"/>
@@ -1381,7 +1379,7 @@
       </c>
     </row>
     <row r="18" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="35"/>
+      <c r="A18" s="41"/>
       <c r="B18" s="17"/>
       <c r="C18" s="21" t="str">
         <f t="shared" si="0"/>
@@ -1419,7 +1417,7 @@
       </c>
     </row>
     <row r="19" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="35"/>
+      <c r="A19" s="41"/>
       <c r="B19" s="17"/>
       <c r="C19" s="21" t="str">
         <f t="shared" si="0"/>
@@ -1457,7 +1455,7 @@
       </c>
     </row>
     <row r="20" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="35"/>
+      <c r="A20" s="41"/>
       <c r="B20" s="17"/>
       <c r="C20" s="21" t="str">
         <f t="shared" si="0"/>
@@ -1495,7 +1493,7 @@
       </c>
     </row>
     <row r="21" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="35"/>
+      <c r="A21" s="41"/>
       <c r="B21" s="17"/>
       <c r="C21" s="21" t="str">
         <f t="shared" si="0"/>
@@ -1533,7 +1531,7 @@
       </c>
     </row>
     <row r="22" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="35"/>
+      <c r="A22" s="41"/>
       <c r="B22" s="17"/>
       <c r="C22" s="21" t="str">
         <f t="shared" si="0"/>
@@ -1571,7 +1569,7 @@
       </c>
     </row>
     <row r="23" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="35"/>
+      <c r="A23" s="41"/>
       <c r="B23" s="17"/>
       <c r="C23" s="21" t="str">
         <f t="shared" si="0"/>
@@ -1609,7 +1607,7 @@
       </c>
     </row>
     <row r="24" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="35"/>
+      <c r="A24" s="41"/>
       <c r="B24" s="17"/>
       <c r="C24" s="21" t="str">
         <f t="shared" si="0"/>
@@ -1647,7 +1645,7 @@
       </c>
     </row>
     <row r="25" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="35"/>
+      <c r="A25" s="41"/>
       <c r="B25" s="17"/>
       <c r="C25" s="21" t="str">
         <f t="shared" si="0"/>
@@ -1685,7 +1683,7 @@
       </c>
     </row>
     <row r="26" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="35"/>
+      <c r="A26" s="41"/>
       <c r="B26" s="17"/>
       <c r="C26" s="21" t="str">
         <f t="shared" si="0"/>
@@ -1723,7 +1721,7 @@
       </c>
     </row>
     <row r="27" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="35"/>
+      <c r="A27" s="41"/>
       <c r="B27" s="17"/>
       <c r="C27" s="21" t="str">
         <f t="shared" si="0"/>
@@ -1761,7 +1759,7 @@
       </c>
     </row>
     <row r="28" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="35"/>
+      <c r="A28" s="41"/>
       <c r="B28" s="17"/>
       <c r="C28" s="21" t="str">
         <f t="shared" si="0"/>
@@ -1799,7 +1797,7 @@
       </c>
     </row>
     <row r="29" spans="1:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="35"/>
+      <c r="A29" s="41"/>
       <c r="B29" s="17"/>
       <c r="C29" s="21" t="str">
         <f t="shared" si="0"/>
@@ -1847,53 +1845,53 @@
       <c r="H30" s="26"/>
     </row>
     <row r="31" spans="1:15" s="8" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="36" t="s">
+      <c r="A31" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B31" s="36"/>
-      <c r="C31" s="36"/>
-      <c r="D31" s="36"/>
-      <c r="E31" s="36"/>
-      <c r="F31" s="36"/>
-      <c r="G31" s="36"/>
-      <c r="H31" s="36"/>
-      <c r="I31" s="36"/>
-      <c r="J31" s="36"/>
-      <c r="K31" s="36"/>
-      <c r="L31" s="36"/>
-      <c r="M31" s="36"/>
+      <c r="B31" s="42"/>
+      <c r="C31" s="42"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="42"/>
+      <c r="F31" s="42"/>
+      <c r="G31" s="42"/>
+      <c r="H31" s="42"/>
+      <c r="I31" s="42"/>
+      <c r="J31" s="42"/>
+      <c r="K31" s="42"/>
+      <c r="L31" s="42"/>
+      <c r="M31" s="42"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A33" s="37" t="s">
+      <c r="A33" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B33" s="37"/>
-      <c r="C33" s="37"/>
-      <c r="D33" s="37"/>
-      <c r="E33" s="37"/>
-      <c r="F33" s="37"/>
-      <c r="G33" s="37"/>
-      <c r="H33" s="37"/>
-      <c r="I33" s="37"/>
-      <c r="J33" s="37"/>
-      <c r="K33" s="37"/>
-      <c r="L33" s="37"/>
-      <c r="M33" s="37"/>
+      <c r="B33" s="43"/>
+      <c r="C33" s="43"/>
+      <c r="D33" s="43"/>
+      <c r="E33" s="43"/>
+      <c r="F33" s="43"/>
+      <c r="G33" s="43"/>
+      <c r="H33" s="43"/>
+      <c r="I33" s="43"/>
+      <c r="J33" s="43"/>
+      <c r="K33" s="43"/>
+      <c r="L33" s="43"/>
+      <c r="M33" s="43"/>
       <c r="N33" s="7"/>
       <c r="O33" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A7:A29"/>
+    <mergeCell ref="A31:M31"/>
+    <mergeCell ref="A33:M33"/>
+    <mergeCell ref="N5:O5"/>
     <mergeCell ref="A3:O3"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="L5:M5"/>
-    <mergeCell ref="A7:A29"/>
-    <mergeCell ref="A31:M31"/>
-    <mergeCell ref="A33:M33"/>
-    <mergeCell ref="N5:O5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1904,9 +1902,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="96" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:XFD31"/>
-    </sheetView>
+    <sheetView zoomScale="96" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1939,23 +1935,23 @@
       </c>
     </row>
     <row r="3" spans="1:15" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43"/>
-      <c r="M3" s="43"/>
-      <c r="N3" s="43"/>
-      <c r="O3" s="43"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="46"/>
+      <c r="M3" s="46"/>
+      <c r="N3" s="46"/>
+      <c r="O3" s="46"/>
     </row>
     <row r="4" spans="1:15" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
@@ -1964,30 +1960,30 @@
       <c r="A5" s="5"/>
       <c r="B5" s="15"/>
       <c r="C5" s="19"/>
-      <c r="D5" s="41" t="s">
+      <c r="D5" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="42"/>
-      <c r="F5" s="41" t="s">
+      <c r="E5" s="40"/>
+      <c r="F5" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="42"/>
-      <c r="H5" s="41" t="s">
+      <c r="G5" s="40"/>
+      <c r="H5" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="42"/>
-      <c r="J5" s="41" t="s">
+      <c r="I5" s="40"/>
+      <c r="J5" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="42"/>
-      <c r="L5" s="41" t="s">
+      <c r="K5" s="40"/>
+      <c r="L5" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="M5" s="42"/>
-      <c r="N5" s="38" t="s">
+      <c r="M5" s="40"/>
+      <c r="N5" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="O5" s="39"/>
+      <c r="O5" s="45"/>
     </row>
     <row r="6" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="16" t="s">
@@ -2034,7 +2030,7 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="35"/>
+      <c r="A7" s="41"/>
       <c r="B7" s="17"/>
       <c r="C7" s="21" t="str">
         <f>IF(ISBLANK($B7),"",SUM(D7,F7,H7,J7,L7,N7))</f>
@@ -2072,7 +2068,7 @@
       </c>
     </row>
     <row r="8" spans="1:15" s="7" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="35"/>
+      <c r="A8" s="41"/>
       <c r="B8" s="17"/>
       <c r="C8" s="21" t="str">
         <f t="shared" ref="C8:C29" si="0">IF(ISBLANK($B8),"",SUM(D8,F8,H8,J8,L8,N8))</f>
@@ -2110,7 +2106,7 @@
       </c>
     </row>
     <row r="9" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="35"/>
+      <c r="A9" s="41"/>
       <c r="B9" s="17"/>
       <c r="C9" s="21" t="str">
         <f t="shared" si="0"/>
@@ -2148,7 +2144,7 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="35"/>
+      <c r="A10" s="41"/>
       <c r="B10" s="17"/>
       <c r="C10" s="21" t="str">
         <f t="shared" si="0"/>
@@ -2186,7 +2182,7 @@
       </c>
     </row>
     <row r="11" spans="1:15" s="7" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="35"/>
+      <c r="A11" s="41"/>
       <c r="B11" s="17"/>
       <c r="C11" s="21" t="str">
         <f t="shared" si="0"/>
@@ -2224,7 +2220,7 @@
       </c>
     </row>
     <row r="12" spans="1:15" s="7" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="35"/>
+      <c r="A12" s="41"/>
       <c r="B12" s="17"/>
       <c r="C12" s="21" t="str">
         <f t="shared" si="0"/>
@@ -2262,7 +2258,7 @@
       </c>
     </row>
     <row r="13" spans="1:15" s="7" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="35"/>
+      <c r="A13" s="41"/>
       <c r="B13" s="17"/>
       <c r="C13" s="21" t="str">
         <f t="shared" si="0"/>
@@ -2300,7 +2296,7 @@
       </c>
     </row>
     <row r="14" spans="1:15" s="7" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="35"/>
+      <c r="A14" s="41"/>
       <c r="B14" s="17"/>
       <c r="C14" s="21" t="str">
         <f t="shared" si="0"/>
@@ -2338,7 +2334,7 @@
       </c>
     </row>
     <row r="15" spans="1:15" s="7" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="35"/>
+      <c r="A15" s="41"/>
       <c r="B15" s="17"/>
       <c r="C15" s="21" t="str">
         <f t="shared" si="0"/>
@@ -2376,7 +2372,7 @@
       </c>
     </row>
     <row r="16" spans="1:15" s="7" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="35"/>
+      <c r="A16" s="41"/>
       <c r="B16" s="17"/>
       <c r="C16" s="21" t="str">
         <f t="shared" si="0"/>
@@ -2414,7 +2410,7 @@
       </c>
     </row>
     <row r="17" spans="1:15" s="7" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="35"/>
+      <c r="A17" s="41"/>
       <c r="B17" s="17"/>
       <c r="C17" s="21" t="str">
         <f t="shared" si="0"/>
@@ -2452,7 +2448,7 @@
       </c>
     </row>
     <row r="18" spans="1:15" s="7" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="35"/>
+      <c r="A18" s="41"/>
       <c r="B18" s="17"/>
       <c r="C18" s="21" t="str">
         <f t="shared" si="0"/>
@@ -2490,7 +2486,7 @@
       </c>
     </row>
     <row r="19" spans="1:15" s="7" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="35"/>
+      <c r="A19" s="41"/>
       <c r="B19" s="17"/>
       <c r="C19" s="21" t="str">
         <f t="shared" si="0"/>
@@ -2528,7 +2524,7 @@
       </c>
     </row>
     <row r="20" spans="1:15" s="7" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="35"/>
+      <c r="A20" s="41"/>
       <c r="B20" s="17"/>
       <c r="C20" s="21" t="str">
         <f t="shared" si="0"/>
@@ -2566,7 +2562,7 @@
       </c>
     </row>
     <row r="21" spans="1:15" s="7" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="35"/>
+      <c r="A21" s="41"/>
       <c r="B21" s="17"/>
       <c r="C21" s="21" t="str">
         <f t="shared" si="0"/>
@@ -2604,7 +2600,7 @@
       </c>
     </row>
     <row r="22" spans="1:15" s="7" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="35"/>
+      <c r="A22" s="41"/>
       <c r="B22" s="17"/>
       <c r="C22" s="21" t="str">
         <f t="shared" si="0"/>
@@ -2642,7 +2638,7 @@
       </c>
     </row>
     <row r="23" spans="1:15" s="7" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="35"/>
+      <c r="A23" s="41"/>
       <c r="B23" s="17"/>
       <c r="C23" s="21" t="str">
         <f t="shared" si="0"/>
@@ -2680,7 +2676,7 @@
       </c>
     </row>
     <row r="24" spans="1:15" s="7" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="35"/>
+      <c r="A24" s="41"/>
       <c r="B24" s="17"/>
       <c r="C24" s="21" t="str">
         <f t="shared" si="0"/>
@@ -2718,7 +2714,7 @@
       </c>
     </row>
     <row r="25" spans="1:15" s="7" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="35"/>
+      <c r="A25" s="41"/>
       <c r="B25" s="17"/>
       <c r="C25" s="21" t="str">
         <f t="shared" si="0"/>
@@ -2756,7 +2752,7 @@
       </c>
     </row>
     <row r="26" spans="1:15" s="7" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="35"/>
+      <c r="A26" s="41"/>
       <c r="B26" s="17"/>
       <c r="C26" s="21" t="str">
         <f t="shared" si="0"/>
@@ -2794,7 +2790,7 @@
       </c>
     </row>
     <row r="27" spans="1:15" s="7" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="35"/>
+      <c r="A27" s="41"/>
       <c r="B27" s="17"/>
       <c r="C27" s="21" t="str">
         <f t="shared" si="0"/>
@@ -2832,7 +2828,7 @@
       </c>
     </row>
     <row r="28" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="35"/>
+      <c r="A28" s="41"/>
       <c r="B28" s="17"/>
       <c r="C28" s="21" t="str">
         <f t="shared" si="0"/>
@@ -2870,7 +2866,7 @@
       </c>
     </row>
     <row r="29" spans="1:15" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="35"/>
+      <c r="A29" s="41"/>
       <c r="B29" s="17"/>
       <c r="C29" s="21" t="str">
         <f t="shared" si="0"/>
@@ -2925,40 +2921,40 @@
       <c r="O30" s="10"/>
     </row>
     <row r="31" spans="1:15" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="36" t="s">
+      <c r="A31" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B31" s="36"/>
-      <c r="C31" s="36"/>
-      <c r="D31" s="36"/>
-      <c r="E31" s="36"/>
-      <c r="F31" s="36"/>
-      <c r="G31" s="36"/>
-      <c r="H31" s="36"/>
-      <c r="I31" s="36"/>
-      <c r="J31" s="36"/>
-      <c r="K31" s="36"/>
-      <c r="L31" s="36"/>
-      <c r="M31" s="36"/>
+      <c r="B31" s="42"/>
+      <c r="C31" s="42"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="42"/>
+      <c r="F31" s="42"/>
+      <c r="G31" s="42"/>
+      <c r="H31" s="42"/>
+      <c r="I31" s="42"/>
+      <c r="J31" s="42"/>
+      <c r="K31" s="42"/>
+      <c r="L31" s="42"/>
+      <c r="M31" s="42"/>
       <c r="N31" s="8"/>
       <c r="O31" s="8"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A33" s="37" t="s">
+      <c r="A33" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B33" s="37"/>
-      <c r="C33" s="37"/>
-      <c r="D33" s="37"/>
-      <c r="E33" s="37"/>
-      <c r="F33" s="37"/>
-      <c r="G33" s="37"/>
-      <c r="H33" s="37"/>
-      <c r="I33" s="37"/>
-      <c r="J33" s="37"/>
-      <c r="K33" s="37"/>
-      <c r="L33" s="37"/>
-      <c r="M33" s="37"/>
+      <c r="B33" s="43"/>
+      <c r="C33" s="43"/>
+      <c r="D33" s="43"/>
+      <c r="E33" s="43"/>
+      <c r="F33" s="43"/>
+      <c r="G33" s="43"/>
+      <c r="H33" s="43"/>
+      <c r="I33" s="43"/>
+      <c r="J33" s="43"/>
+      <c r="K33" s="43"/>
+      <c r="L33" s="43"/>
+      <c r="M33" s="43"/>
       <c r="N33" s="7"/>
       <c r="O33" s="7"/>
     </row>
@@ -2984,9 +2980,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12253E63-19A0-4D98-92C0-18466B6DE8AE}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3007,296 +3001,296 @@
       <c r="A2" s="5"/>
     </row>
     <row r="3" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
     </row>
     <row r="4" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="45" t="s">
+      <c r="D5" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="45" t="s">
+      <c r="E5" s="36" t="s">
         <v>22</v>
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
     </row>
     <row r="6" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="35"/>
+      <c r="A6" s="41"/>
       <c r="B6" s="17"/>
-      <c r="C6" s="46" t="str">
+      <c r="C6" s="37" t="str">
         <f>IF(ISBLANK($B6),"",SUM(D6,E6,#REF!,#REF!,#REF!,#REF!))</f>
         <v/>
       </c>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
     </row>
     <row r="7" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="35"/>
+      <c r="A7" s="41"/>
       <c r="B7" s="17"/>
-      <c r="C7" s="46" t="str">
+      <c r="C7" s="37" t="str">
         <f>IF(ISBLANK($B7),"",SUM(D7,E7,#REF!,#REF!,#REF!,#REF!))</f>
         <v/>
       </c>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
     </row>
     <row r="8" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="35"/>
+      <c r="A8" s="41"/>
       <c r="B8" s="17"/>
-      <c r="C8" s="46" t="str">
+      <c r="C8" s="37" t="str">
         <f>IF(ISBLANK($B8),"",SUM(D8,E8,#REF!,#REF!,#REF!,#REF!))</f>
         <v/>
       </c>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
     </row>
     <row r="9" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="35"/>
+      <c r="A9" s="41"/>
       <c r="B9" s="17"/>
-      <c r="C9" s="46" t="str">
+      <c r="C9" s="37" t="str">
         <f>IF(ISBLANK($B9),"",SUM(D9,E9,#REF!,#REF!,#REF!,#REF!))</f>
         <v/>
       </c>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
     </row>
     <row r="10" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="35"/>
+      <c r="A10" s="41"/>
       <c r="B10" s="17"/>
-      <c r="C10" s="46" t="str">
+      <c r="C10" s="37" t="str">
         <f>IF(ISBLANK($B10),"",SUM(D10,E10,#REF!,#REF!,#REF!,#REF!))</f>
         <v/>
       </c>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
     </row>
     <row r="11" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="35"/>
+      <c r="A11" s="41"/>
       <c r="B11" s="17"/>
-      <c r="C11" s="46" t="str">
+      <c r="C11" s="37" t="str">
         <f>IF(ISBLANK($B11),"",SUM(D11,E11,#REF!,#REF!,#REF!,#REF!))</f>
         <v/>
       </c>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
     </row>
     <row r="12" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="35"/>
+      <c r="A12" s="41"/>
       <c r="B12" s="17"/>
-      <c r="C12" s="46" t="str">
+      <c r="C12" s="37" t="str">
         <f>IF(ISBLANK($B12),"",SUM(D12,E12,#REF!,#REF!,#REF!,#REF!))</f>
         <v/>
       </c>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
     </row>
     <row r="13" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="35"/>
+      <c r="A13" s="41"/>
       <c r="B13" s="17"/>
-      <c r="C13" s="46" t="str">
+      <c r="C13" s="37" t="str">
         <f>IF(ISBLANK($B13),"",SUM(D13,E13,#REF!,#REF!,#REF!,#REF!))</f>
         <v/>
       </c>
-      <c r="D13" s="46"/>
-      <c r="E13" s="46"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
     </row>
     <row r="14" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="35"/>
+      <c r="A14" s="41"/>
       <c r="B14" s="17"/>
-      <c r="C14" s="46" t="str">
+      <c r="C14" s="37" t="str">
         <f>IF(ISBLANK($B14),"",SUM(D14,E14,#REF!,#REF!,#REF!,#REF!))</f>
         <v/>
       </c>
-      <c r="D14" s="46"/>
-      <c r="E14" s="46"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
     </row>
     <row r="15" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="35"/>
+      <c r="A15" s="41"/>
       <c r="B15" s="17"/>
-      <c r="C15" s="46" t="str">
+      <c r="C15" s="37" t="str">
         <f>IF(ISBLANK($B15),"",SUM(D15,E15,#REF!,#REF!,#REF!,#REF!))</f>
         <v/>
       </c>
-      <c r="D15" s="46"/>
-      <c r="E15" s="46"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
     </row>
     <row r="16" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="35"/>
+      <c r="A16" s="41"/>
       <c r="B16" s="17"/>
-      <c r="C16" s="46" t="str">
+      <c r="C16" s="37" t="str">
         <f>IF(ISBLANK($B16),"",SUM(D16,E16,#REF!,#REF!,#REF!,#REF!))</f>
         <v/>
       </c>
-      <c r="D16" s="46"/>
-      <c r="E16" s="46"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
     </row>
     <row r="17" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="35"/>
+      <c r="A17" s="41"/>
       <c r="B17" s="17"/>
-      <c r="C17" s="46" t="str">
+      <c r="C17" s="37" t="str">
         <f>IF(ISBLANK($B17),"",SUM(D17,E17,#REF!,#REF!,#REF!,#REF!))</f>
         <v/>
       </c>
-      <c r="D17" s="46"/>
-      <c r="E17" s="46"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
     </row>
     <row r="18" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="35"/>
+      <c r="A18" s="41"/>
       <c r="B18" s="17"/>
-      <c r="C18" s="46" t="str">
+      <c r="C18" s="37" t="str">
         <f>IF(ISBLANK($B18),"",SUM(D18,E18,#REF!,#REF!,#REF!,#REF!))</f>
         <v/>
       </c>
-      <c r="D18" s="46"/>
-      <c r="E18" s="46"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
     </row>
     <row r="19" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="35"/>
+      <c r="A19" s="41"/>
       <c r="B19" s="17"/>
-      <c r="C19" s="46" t="str">
+      <c r="C19" s="37" t="str">
         <f>IF(ISBLANK($B19),"",SUM(D19,E19,#REF!,#REF!,#REF!,#REF!))</f>
         <v/>
       </c>
-      <c r="D19" s="46"/>
-      <c r="E19" s="46"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
     </row>
     <row r="20" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="35"/>
+      <c r="A20" s="41"/>
       <c r="B20" s="17"/>
-      <c r="C20" s="46" t="str">
+      <c r="C20" s="37" t="str">
         <f>IF(ISBLANK($B20),"",SUM(D20,E20,#REF!,#REF!,#REF!,#REF!))</f>
         <v/>
       </c>
-      <c r="D20" s="46"/>
-      <c r="E20" s="46"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="37"/>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
     </row>
     <row r="21" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="35"/>
+      <c r="A21" s="41"/>
       <c r="B21" s="17"/>
-      <c r="C21" s="46" t="str">
+      <c r="C21" s="37" t="str">
         <f>IF(ISBLANK($B21),"",SUM(D21,E21,#REF!,#REF!,#REF!,#REF!))</f>
         <v/>
       </c>
-      <c r="D21" s="46"/>
-      <c r="E21" s="46"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="37"/>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
     </row>
     <row r="22" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="35"/>
+      <c r="A22" s="41"/>
       <c r="B22" s="17"/>
-      <c r="C22" s="46" t="str">
+      <c r="C22" s="37" t="str">
         <f>IF(ISBLANK($B22),"",SUM(D22,E22,#REF!,#REF!,#REF!,#REF!))</f>
         <v/>
       </c>
-      <c r="D22" s="46"/>
-      <c r="E22" s="46"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="37"/>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
     </row>
     <row r="23" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="35"/>
+      <c r="A23" s="41"/>
       <c r="B23" s="17"/>
-      <c r="C23" s="46" t="str">
+      <c r="C23" s="37" t="str">
         <f>IF(ISBLANK($B23),"",SUM(D23,E23,#REF!,#REF!,#REF!,#REF!))</f>
         <v/>
       </c>
-      <c r="D23" s="46"/>
-      <c r="E23" s="46"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="37"/>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
     </row>
     <row r="24" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="35"/>
+      <c r="A24" s="41"/>
       <c r="B24" s="17"/>
-      <c r="C24" s="46" t="str">
+      <c r="C24" s="37" t="str">
         <f>IF(ISBLANK($B24),"",SUM(D24,E24,#REF!,#REF!,#REF!,#REF!))</f>
         <v/>
       </c>
-      <c r="D24" s="46"/>
-      <c r="E24" s="46"/>
+      <c r="D24" s="37"/>
+      <c r="E24" s="37"/>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
     </row>
     <row r="25" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="35"/>
+      <c r="A25" s="41"/>
       <c r="B25" s="17"/>
-      <c r="C25" s="46" t="str">
+      <c r="C25" s="37" t="str">
         <f>IF(ISBLANK($B25),"",SUM(D25,E25,#REF!,#REF!,#REF!,#REF!))</f>
         <v/>
       </c>
-      <c r="D25" s="46"/>
-      <c r="E25" s="46"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="37"/>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
     </row>
     <row r="26" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="35"/>
+      <c r="A26" s="41"/>
       <c r="B26" s="17"/>
-      <c r="C26" s="46" t="str">
+      <c r="C26" s="37" t="str">
         <f>IF(ISBLANK($B26),"",SUM(D26,E26,#REF!,#REF!,#REF!,#REF!))</f>
         <v/>
       </c>
-      <c r="D26" s="46"/>
-      <c r="E26" s="46"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="37"/>
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
     </row>
     <row r="27" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="35"/>
+      <c r="A27" s="41"/>
       <c r="B27" s="17"/>
-      <c r="C27" s="46" t="str">
+      <c r="C27" s="37" t="str">
         <f>IF(ISBLANK($B27),"",SUM(D27,E27,#REF!,#REF!,#REF!,#REF!))</f>
         <v/>
       </c>
-      <c r="D27" s="46"/>
-      <c r="E27" s="46"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
     </row>
@@ -3310,26 +3304,26 @@
       <c r="G28" s="26"/>
     </row>
     <row r="29" spans="1:7" s="8" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="36" t="s">
+      <c r="A29" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B29" s="36"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="36"/>
-      <c r="E29" s="36"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="36"/>
+      <c r="B29" s="42"/>
+      <c r="C29" s="42"/>
+      <c r="D29" s="42"/>
+      <c r="E29" s="42"/>
+      <c r="F29" s="42"/>
+      <c r="G29" s="42"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="37" t="s">
+      <c r="A31" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="37"/>
-      <c r="C31" s="37"/>
-      <c r="D31" s="37"/>
-      <c r="E31" s="37"/>
-      <c r="F31" s="37"/>
-      <c r="G31" s="37"/>
+      <c r="B31" s="43"/>
+      <c r="C31" s="43"/>
+      <c r="D31" s="43"/>
+      <c r="E31" s="43"/>
+      <c r="F31" s="43"/>
+      <c r="G31" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>